<commit_message>
Cleaned up the code and added meaningful comments for documentation
</commit_message>
<xml_diff>
--- a/ticket_counts.xlsx
+++ b/ticket_counts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2976,10 +2976,8 @@
           <t>Chris Gallinger-Long</t>
         </is>
       </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>145</t>
-        </is>
+      <c r="B170" t="n">
+        <v>145</v>
       </c>
       <c r="C170" t="inlineStr">
         <is>
@@ -2993,10 +2991,8 @@
           <t>Jamison Golec</t>
         </is>
       </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>115</t>
-        </is>
+      <c r="B171" t="n">
+        <v>115</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
@@ -3010,10 +3006,8 @@
           <t>Leo Himstreet</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="B172" t="n">
+        <v>90</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
@@ -3027,10 +3021,8 @@
           <t>Bella Lyon</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>87</t>
-        </is>
+      <c r="B173" t="n">
+        <v>87</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
@@ -3044,10 +3036,8 @@
           <t>Dylan Squires</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
+      <c r="B174" t="n">
+        <v>52</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
@@ -3061,10 +3051,8 @@
           <t>Gabriella Puentes-Gray</t>
         </is>
       </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
+      <c r="B175" t="n">
+        <v>42</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
@@ -3078,10 +3066,8 @@
           <t>Max Kellogg</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="B176" t="n">
+        <v>40</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -3095,10 +3081,8 @@
           <t>Mackenzie Pelson</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="B177" t="n">
+        <v>33</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -3112,10 +3096,8 @@
           <t>Miles Anderson</t>
         </is>
       </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="B178" t="n">
+        <v>30</v>
       </c>
       <c r="C178" t="inlineStr">
         <is>
@@ -3129,10 +3111,8 @@
           <t>Alexia Crawford</t>
         </is>
       </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="B179" t="n">
+        <v>25</v>
       </c>
       <c r="C179" t="inlineStr">
         <is>
@@ -3146,10 +3126,8 @@
           <t>Charlie Maher</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="B180" t="n">
+        <v>25</v>
       </c>
       <c r="C180" t="inlineStr">
         <is>
@@ -3163,10 +3141,8 @@
           <t>Liam Sack</t>
         </is>
       </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="B181" t="n">
+        <v>25</v>
       </c>
       <c r="C181" t="inlineStr">
         <is>
@@ -3180,10 +3156,8 @@
           <t>Ryan Hood</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="B182" t="n">
+        <v>22</v>
       </c>
       <c r="C182" t="inlineStr">
         <is>
@@ -3197,10 +3171,8 @@
           <t>Alma Zapien</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B183" t="n">
+        <v>20</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
@@ -3214,10 +3186,8 @@
           <t>Max Barnett</t>
         </is>
       </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="B184" t="n">
+        <v>19</v>
       </c>
       <c r="C184" t="inlineStr">
         <is>
@@ -3231,10 +3201,8 @@
           <t>Andrew Garcia</t>
         </is>
       </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B185" t="n">
+        <v>16</v>
       </c>
       <c r="C185" t="inlineStr">
         <is>
@@ -3248,10 +3216,8 @@
           <t>Sean Lin</t>
         </is>
       </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="B186" t="n">
+        <v>15</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
@@ -3265,10 +3231,8 @@
           <t>Jessie Schwartz</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="B187" t="n">
+        <v>14</v>
       </c>
       <c r="C187" t="inlineStr">
         <is>
@@ -3282,10 +3246,8 @@
           <t>Nithi Deivanayagam</t>
         </is>
       </c>
-      <c r="B188" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="B188" t="n">
+        <v>13</v>
       </c>
       <c r="C188" t="inlineStr">
         <is>
@@ -3299,10 +3261,8 @@
           <t>David Wagner</t>
         </is>
       </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B189" t="n">
+        <v>11</v>
       </c>
       <c r="C189" t="inlineStr">
         <is>
@@ -3316,10 +3276,8 @@
           <t>Robert Bennett</t>
         </is>
       </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="B190" t="n">
+        <v>9</v>
       </c>
       <c r="C190" t="inlineStr">
         <is>
@@ -3333,10 +3291,8 @@
           <t>Parker Lemme</t>
         </is>
       </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="B191" t="n">
+        <v>9</v>
       </c>
       <c r="C191" t="inlineStr">
         <is>
@@ -3350,10 +3306,8 @@
           <t>Tyler Payne</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="B192" t="n">
+        <v>6</v>
       </c>
       <c r="C192" t="inlineStr">
         <is>
@@ -3367,10 +3321,8 @@
           <t>Jonah Olin</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="B193" t="n">
+        <v>4</v>
       </c>
       <c r="C193" t="inlineStr">
         <is>
@@ -3384,10 +3336,8 @@
           <t>Katie Harsh</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="B194" t="n">
+        <v>4</v>
       </c>
       <c r="C194" t="inlineStr">
         <is>
@@ -3401,10 +3351,8 @@
           <t>Alice Brown</t>
         </is>
       </c>
-      <c r="B195" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="B195" t="n">
+        <v>4</v>
       </c>
       <c r="C195" t="inlineStr">
         <is>
@@ -3418,10 +3366,8 @@
           <t>Maxine Bays</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="B196" t="n">
+        <v>3</v>
       </c>
       <c r="C196" t="inlineStr">
         <is>
@@ -3435,14 +3381,2168 @@
           <t>Sara Stubbs</t>
         </is>
       </c>
-      <c r="B197" t="inlineStr">
+      <c r="B197" t="n">
+        <v>1</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>2025-04-24 23:00:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Chris Gallinger-Long</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>145</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Jamison Golec</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>115</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Leo Himstreet</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>90</v>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Bella Lyon</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>87</v>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Dylan Squires</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>52</v>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Gabriella Puentes-Gray</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>42</v>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Max Kellogg</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>40</v>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Mackenzie Pelson</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>33</v>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Miles Anderson</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>30</v>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Alexia Crawford</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>25</v>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Charlie Maher</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>25</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Liam Sack</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>25</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Ryan Hood</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>22</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Alma Zapien</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>20</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Max Barnett</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>19</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Andrew Garcia</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>16</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Sean Lin</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>14</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Jessie Schwartz</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>14</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Nithi Deivanayagam</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>13</v>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>David Wagner</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>11</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Robert Bennett</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>9</v>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Parker Lemme</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>9</v>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Tyler Payne</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>7</v>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Jonah Olin</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>4</v>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Katie Harsh</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>4</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Alice Brown</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>4</v>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Maxine Bays</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>3</v>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Sara Stubbs</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>1</v>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>2025-04-25 08:48:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Chris Gallinger-Long</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>145</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Jamison Golec</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>115</v>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Leo Himstreet</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>90</v>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Bella Lyon</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>87</v>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Dylan Squires</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>52</v>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Gabriella Puentes-Gray</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>42</v>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Max Kellogg</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>40</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Mackenzie Pelson</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>33</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Miles Anderson</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>30</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Alexia Crawford</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>25</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Charlie Maher</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>25</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Liam Sack</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>25</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Ryan Hood</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>22</v>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Alma Zapien</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>20</v>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Max Barnett</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>19</v>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Andrew Garcia</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>16</v>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Sean Lin</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>14</v>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Jessie Schwartz</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>14</v>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Nithi Deivanayagam</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>13</v>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>David Wagner</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>11</v>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Robert Bennett</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>9</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Parker Lemme</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>9</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Tyler Payne</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>7</v>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Jonah Olin</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>4</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Katie Harsh</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>4</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Alice Brown</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>4</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Maxine Bays</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>3</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Sara Stubbs</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>1</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>2025-04-25 09:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Chris Gallinger-Long</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>145</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Jamison Golec</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>115</v>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Leo Himstreet</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>90</v>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Bella Lyon</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>87</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Dylan Squires</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>52</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Gabriella Puentes-Gray</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>42</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Max Kellogg</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>40</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Mackenzie Pelson</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>33</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Miles Anderson</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>30</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Alexia Crawford</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>25</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Charlie Maher</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>25</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Liam Sack</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>25</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Ryan Hood</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>22</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Alma Zapien</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>20</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Max Barnett</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>19</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Andrew Garcia</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>16</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Sean Lin</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>14</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Jessie Schwartz</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>14</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Nithi Deivanayagam</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>13</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>David Wagner</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>11</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Robert Bennett</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>9</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Parker Lemme</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>9</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Tyler Payne</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>8</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Jonah Olin</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>4</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Katie Harsh</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>4</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Alice Brown</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>4</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Maxine Bays</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>3</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Sara Stubbs</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>1</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:00:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Chris Gallinger-Long</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>145</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Jamison Golec</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>115</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Leo Himstreet</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>90</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Bella Lyon</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>87</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Dylan Squires</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>52</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Gabriella Puentes-Gray</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>42</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Max Kellogg</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>40</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Mackenzie Pelson</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>33</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Miles Anderson</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>30</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Alexia Crawford</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>25</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Charlie Maher</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>25</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Liam Sack</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>25</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Ryan Hood</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>22</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Alma Zapien</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>20</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Max Barnett</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>19</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Andrew Garcia</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>16</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Sean Lin</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>14</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Jessie Schwartz</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>14</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Nithi Deivanayagam</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>13</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>David Wagner</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>11</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Robert Bennett</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>9</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Parker Lemme</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>9</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Tyler Payne</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>8</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Jonah Olin</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>4</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Katie Harsh</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>4</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Alice Brown</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>4</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Maxine Bays</t>
+        </is>
+      </c>
+      <c r="B308" t="n">
+        <v>3</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Sara Stubbs</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>1</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Chris Gallinger-Long</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>147</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Jamison Golec</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Leo Himstreet</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Bella Lyon</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Dylan Squires</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Gabriella Puentes-Gray</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Max Kellogg</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Mackenzie Pelson</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Miles Anderson</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Alexia Crawford</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Charlie Maher</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Liam Sack</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Ryan Hood</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Alma Zapien</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Max Barnett</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Andrew Garcia</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Sean Lin</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Jessie Schwartz</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Nithi Deivanayagam</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>David Wagner</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Robert Bennett</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Parker Lemme</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Tyler Payne</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>Jonah Olin</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Katie Harsh</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Alice Brown</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>Maxine Bays</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>Sara Stubbs</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>2025-04-24 23:00:12</t>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:13</t>
         </is>
       </c>
     </row>

</xml_diff>